<commit_message>
New tiles, unlock action created and tested
</commit_message>
<xml_diff>
--- a/resources/map builder.xlsx
+++ b/resources/map builder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephenBell\.vscode\Python\The Castle\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DC8E9D-27A8-4F58-8900-C5E673BF563D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615A91F-FE16-49DC-A57F-E1BC82FF4638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
+    <workbookView xWindow="3405" yWindow="4095" windowWidth="21600" windowHeight="11295" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
   </bookViews>
   <sheets>
     <sheet name="bf1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
   <si>
     <t>jail_cell</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>five_gold</t>
+  </si>
+  <si>
+    <t>armory</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <dimension ref="D2:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +556,7 @@
         <v>5</v>
       </c>
       <c r="I8" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J8" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
More updates and changes to be worked on.
</commit_message>
<xml_diff>
--- a/resources/map builder.xlsx
+++ b/resources/map builder.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephenBell\.vscode\Python\The Castle\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephenBell\.vscode\Python\The_Castle\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615A91F-FE16-49DC-A57F-E1BC82FF4638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BE305C-2147-4B7F-982C-C6730C535368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="4095" windowWidth="21600" windowHeight="11295" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
   </bookViews>
   <sheets>
     <sheet name="bf1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
   <si>
     <t>jail_cell</t>
   </si>
@@ -75,6 +76,39 @@
   </si>
   <si>
     <t>armory</t>
+  </si>
+  <si>
+    <t>dungeon</t>
+  </si>
+  <si>
+    <t>torture_chamber</t>
+  </si>
+  <si>
+    <t>guard_room</t>
+  </si>
+  <si>
+    <t>giant_centipede_room</t>
+  </si>
+  <si>
+    <t>demon_bat_room</t>
+  </si>
+  <si>
+    <t>skeleton_room</t>
+  </si>
+  <si>
+    <t>empty_hallway</t>
+  </si>
+  <si>
+    <t>large_rat_room</t>
+  </si>
+  <si>
+    <t>pre_flooded_hall</t>
+  </si>
+  <si>
+    <t>flooded_hall</t>
+  </si>
+  <si>
+    <t>ritual_room</t>
   </si>
 </sst>
 </file>
@@ -98,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,12 +140,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BAFD4BA-047E-4AA0-8068-A4084B3B261C}">
   <dimension ref="D2:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -624,4 +676,170 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB6A692-5487-419C-82DD-9ADE5B871C27}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Work done on more map tiles, items, functions
</commit_message>
<xml_diff>
--- a/resources/map builder.xlsx
+++ b/resources/map builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephenBell\.vscode\Python\The_Castle\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BE305C-2147-4B7F-982C-C6730C535368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B37451-FF8F-483C-BAEB-D54A80063BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
   </bookViews>
   <sheets>
     <sheet name="bf1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
   <si>
     <t>jail_cell</t>
   </si>
@@ -78,9 +78,6 @@
     <t>armory</t>
   </si>
   <si>
-    <t>dungeon</t>
-  </si>
-  <si>
     <t>torture_chamber</t>
   </si>
   <si>
@@ -109,6 +106,12 @@
   </si>
   <si>
     <t>ritual_room</t>
+  </si>
+  <si>
+    <t>dungeon_1</t>
+  </si>
+  <si>
+    <t>dungeon_2</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +707,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -725,27 +728,27 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -763,7 +766,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -785,7 +788,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -794,7 +797,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
@@ -809,7 +812,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -817,12 +820,12 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -835,7 +838,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1"/>
     </row>

</xml_diff>

<commit_message>
Various changes and updates
</commit_message>
<xml_diff>
--- a/resources/map builder.xlsx
+++ b/resources/map builder.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephenBell\.vscode\Python\The_Castle\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B37451-FF8F-483C-BAEB-D54A80063BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A4B5D7-0B4C-4859-8854-9645365C3D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
+    <workbookView xWindow="2295" yWindow="3105" windowWidth="21600" windowHeight="11295" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
   </bookViews>
   <sheets>
-    <sheet name="bf1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="bf1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,47 +36,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>jail_cell</t>
   </si>
   <si>
-    <t>jail</t>
-  </si>
-  <si>
     <t>empty_passageway</t>
   </si>
   <si>
     <t>stairs</t>
   </si>
   <si>
-    <t>locked_room</t>
-  </si>
-  <si>
     <t>goblin_room</t>
   </si>
   <si>
     <t>giant_spider_room</t>
   </si>
   <si>
-    <t>key_room</t>
-  </si>
-  <si>
     <t>empty_room</t>
   </si>
   <si>
-    <t>find_rusty_dagger_room</t>
-  </si>
-  <si>
-    <t>find_rusty_shield_room</t>
-  </si>
-  <si>
-    <t>five_gold</t>
-  </si>
-  <si>
-    <t>armory</t>
-  </si>
-  <si>
     <t>torture_chamber</t>
   </si>
   <si>
@@ -112,6 +90,9 @@
   </si>
   <si>
     <t>dungeon_2</t>
+  </si>
+  <si>
+    <t>low_trader</t>
   </si>
 </sst>
 </file>
@@ -135,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -143,30 +124,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,213 +447,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BAFD4BA-047E-4AA0-8068-A4084B3B261C}">
-  <dimension ref="D2:M12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB6A692-5487-419C-82DD-9ADE5B871C27}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,9 +459,9 @@
     <col min="1" max="7" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -705,9 +470,9 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -716,120 +481,122 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -838,7 +605,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1"/>
     </row>

</xml_diff>

<commit_message>
Changes and testing underway
</commit_message>
<xml_diff>
--- a/resources/map builder.xlsx
+++ b/resources/map builder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephenBell\.vscode\Python\The_Castle\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A4B5D7-0B4C-4859-8854-9645365C3D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C307B2-0823-4D29-9DEC-793FC8473420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2295" yWindow="3105" windowWidth="21600" windowHeight="11295" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>jail_cell</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>skeleton_room</t>
-  </si>
-  <si>
-    <t>empty_hallway</t>
   </si>
   <si>
     <t>large_rat_room</t>
@@ -128,12 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +447,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,13 +492,13 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -531,7 +527,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -547,11 +543,10 @@
         <v>4</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -579,7 +574,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -587,12 +582,12 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -605,7 +600,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="1"/>
     </row>

</xml_diff>

<commit_message>
work being done, and files being ignored
</commit_message>
<xml_diff>
--- a/resources/map builder.xlsx
+++ b/resources/map builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephenBell\.vscode\Python\The_Castle\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C307B2-0823-4D29-9DEC-793FC8473420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F86B604-ED0F-4989-B9C2-B0032EFDA50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="3105" windowWidth="21600" windowHeight="11295" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EE01D5F3-3837-4679-9528-E247A5A1F625}"/>
   </bookViews>
   <sheets>
     <sheet name="bf1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>jail_cell</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>low_trader</t>
+  </si>
+  <si>
+    <t>giant_spider_room_2</t>
   </si>
 </sst>
 </file>
@@ -446,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB6A692-5487-419C-82DD-9ADE5B871C27}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1"/>
     </row>

</xml_diff>